<commit_message>
Log4j has been integrated
</commit_message>
<xml_diff>
--- a/src/test/java/DataPackage/Data.xlsx
+++ b/src/test/java/DataPackage/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ZLenovo\Asoftware\VatanBilgisayarCaseStudy\src\test\java\DataPackage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6E6E20-A166-42BC-A13E-4747686121ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E00859-C4C0-47C2-A310-368CA3095638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -368,7 +368,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>